<commit_message>
Added graph functions to graph page
</commit_message>
<xml_diff>
--- a/database/sample_database.xlsx
+++ b/database/sample_database.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>snaks</t>
+          <t>snacks</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -528,21 +528,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>241112</v>
+        <v>241008</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>subcriptions</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="D5" t="n">
+        <v>1200</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>prime</t>
         </is>
       </c>
     </row>
@@ -551,21 +549,21 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>241112</v>
+        <v>241031</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>bills</t>
+          <t>accessories</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>200</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>pen</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added edit function to edit page
</commit_message>
<xml_diff>
--- a/database/sample_database.xlsx
+++ b/database/sample_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,19 +486,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>241102</v>
+        <v>241101</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>electricity bill</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1000</v>
+          <t>bills</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>bill</t>
+          <t>edited</t>
         </is>
       </c>
     </row>
@@ -541,29 +543,6 @@
       <c r="E5" t="inlineStr">
         <is>
           <t>prime</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>241031</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>accessories</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>pen</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added comments to edit page
</commit_message>
<xml_diff>
--- a/database/sample_database.xlsx
+++ b/database/sample_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,35 +514,12 @@
           <t>subcriptions</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+      <c r="D4" t="n">
+        <v>200</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>description</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>7</v>
-      </c>
-      <c r="B5" t="n">
-        <v>241114</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>bills</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>120</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>prime</t>
         </is>
       </c>
     </row>

</xml_diff>